<commit_message>
tot ontbreekt door fout karakter in csv
</commit_message>
<xml_diff>
--- a/src/main/resources/be/vlaanderen/bodemenondergrond/data/id/conceptscheme/eenhedenrelatie/eenhedenrelatie.xlsx
+++ b/src/main/resources/be/vlaanderen/bodemenondergrond/data/id/conceptscheme/eenhedenrelatie/eenhedenrelatie.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I4"/>
+  <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -491,36 +491,65 @@
     </row>
     <row r="4">
       <c r="A4" t="str">
-        <v>https://data.bodemenondergrond.vlaanderen.be/id/conceptscheme/eenhedenrelatie</v>
+        <v>https://data.bodemenondergrond.vlaanderen.be/id/concept/eenhedenrelatie/tot</v>
       </c>
       <c r="B4" t="str">
+        <v>http://www.w3.org/2004/02/skos/core#Concept</v>
+      </c>
+      <c r="C4" t="str">
+        <v>be.vlaanderen.bodemenondergrond.data.id.concept.eenhedenrelatie.tot</v>
+      </c>
+      <c r="D4" t="str">
+        <v>Binnen het aangegeven interval komt een al dan niet volledige opeenvolging van eenheden voor, vanaf de jongste geselecteerde eenheid bovenaan (Lid 1) tot de oudste geselecteerde eenheid onderaan (Lid 2).</v>
+      </c>
+      <c r="E4" t="str">
+        <v>https://data.bodemenondergrond.vlaanderen.be/id/conceptscheme/eenhedenrelatie</v>
+      </c>
+      <c r="F4" t="str">
+        <v>Binnen het aangegeven interval komt een al dan niet volledige opeenvolging van eenheden voor, vanaf de jongste geselecteerde eenheid bovenaan (Lid 1) tot de oudste geselecteerde eenheid onderaan (Lid 2).</v>
+      </c>
+      <c r="G4" t="str">
+        <v>tot</v>
+      </c>
+      <c r="H4" t="str">
+        <v>https://data.bodemenondergrond.vlaanderen.be/id/conceptscheme/eenhedenrelatie</v>
+      </c>
+      <c r="I4" t="str">
+        <v>null</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="str">
+        <v>https://data.bodemenondergrond.vlaanderen.be/id/conceptscheme/eenhedenrelatie</v>
+      </c>
+      <c r="B5" t="str">
         <v>http://www.w3.org/2004/02/skos/core#ConceptScheme</v>
       </c>
-      <c r="C4" t="str">
+      <c r="C5" t="str">
         <v>be.vlaanderen.bodemenondergrond.data.id.conceptscheme.eenhedenrelatie</v>
       </c>
-      <c r="D4" t="str">
-        <v>null</v>
-      </c>
-      <c r="E4" t="str">
-        <v>null</v>
-      </c>
-      <c r="F4" t="str">
-        <v>null</v>
-      </c>
-      <c r="G4" t="str">
+      <c r="D5" t="str">
+        <v>null</v>
+      </c>
+      <c r="E5" t="str">
+        <v>null</v>
+      </c>
+      <c r="F5" t="str">
+        <v>null</v>
+      </c>
+      <c r="G5" t="str">
         <v>Lijst van mogelijke relaties tussen eenheden binnen een aangegeven interval</v>
       </c>
-      <c r="H4" t="str">
-        <v>null</v>
-      </c>
-      <c r="I4" t="str">
-        <v>https://data.bodemenondergrond.vlaanderen.be/id/concept/eenhedenrelatie/en|https://data.bodemenondergrond.vlaanderen.be/id/concept/eenhedenrelatie/of</v>
+      <c r="H5" t="str">
+        <v>null</v>
+      </c>
+      <c r="I5" t="str">
+        <v>https://data.bodemenondergrond.vlaanderen.be/id/concept/eenhedenrelatie/en|https://data.bodemenondergrond.vlaanderen.be/id/concept/eenhedenrelatie/of|https://data.bodemenondergrond.vlaanderen.be/id/concept/eenhedenrelatie/tot</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:I4"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:I5"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>